<commit_message>
Add group members github usernames
</commit_message>
<xml_diff>
--- a/_Group Projects/Econ490_groupinfo.xlsx
+++ b/_Group Projects/Econ490_groupinfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20389"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ah1152\Desktop\week3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bl517\Documents\Github\econ490-fall22\_Group Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{638F0EEB-AF13-4425-A65F-F2036960316C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73D1E69B-1FFA-4E8E-9ABB-E6D728C2F416}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7310" windowHeight="6910" xr2:uid="{58429A20-B2A9-4295-BFAA-E668685E1957}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7305" windowHeight="6915" xr2:uid="{58429A20-B2A9-4295-BFAA-E668685E1957}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Acharya, Shaily</t>
   </si>
@@ -82,6 +82,57 @@
   </si>
   <si>
     <t>Smith, Noah B.</t>
+  </si>
+  <si>
+    <t>Github username</t>
+  </si>
+  <si>
+    <t>shailyacharya</t>
+  </si>
+  <si>
+    <t>sbrown5x</t>
+  </si>
+  <si>
+    <t>neeldesai01</t>
+  </si>
+  <si>
+    <t>yc577</t>
+  </si>
+  <si>
+    <t>yashdhuldhoya</t>
+  </si>
+  <si>
+    <t>felipegermanos</t>
+  </si>
+  <si>
+    <t>MoatazGU</t>
+  </si>
+  <si>
+    <t>MarineAntonio</t>
+  </si>
+  <si>
+    <t>FegorEO</t>
+  </si>
+  <si>
+    <t>abigailorbe</t>
+  </si>
+  <si>
+    <t>geena-panzitta</t>
+  </si>
+  <si>
+    <t>bp557</t>
+  </si>
+  <si>
+    <t>AaronShtilerman</t>
+  </si>
+  <si>
+    <t>MiglePetrou</t>
+  </si>
+  <si>
+    <t>Benjamin-Tu</t>
+  </si>
+  <si>
+    <t>f2pHgty8hw</t>
   </si>
 </sst>
 </file>
@@ -476,152 +527,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFEBD00-88FE-43DF-917F-49D058D1B206}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.1796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C2" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C3" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="3">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C9" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C10" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C12" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C14" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C15" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="3">
         <v>5</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>